<commit_message>
第九次提交： 讲解式封装requests samples/requests_utils.py 三层的方式封装get/post request step_request 接口关联： jsonpath re模块：详细讲解
</commit_message>
<xml_diff>
--- a/test_data/test_case.xlsx
+++ b/test_data/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm\API_TEST_FRAME\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB36C6-3516-4A72-AC76-0B806A641DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A62A10B-DF69-4DDA-AE4C-62FD13B87A55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>请求地址</t>
   </si>
   <si>
-    <t>请求参数(get)</t>
-  </si>
-  <si>
     <t>取值方式</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>测试用例步骤</t>
   </si>
   <si>
-    <t>提交数据（post）</t>
-  </si>
-  <si>
     <t>传值变量</t>
   </si>
   <si>
@@ -137,34 +131,43 @@
     <t>{"access_token":${token}}</t>
   </si>
   <si>
+    <t>json键值对</t>
+  </si>
+  <si>
+    <t>{"errcode":45158}</t>
+  </si>
+  <si>
+    <t>case03</t>
+  </si>
+  <si>
+    <t>测试能否正确删除用户标签</t>
+  </si>
+  <si>
+    <t>删除标签接口</t>
+  </si>
+  <si>
+    <t>/cgi-bin/tags/delete</t>
+  </si>
+  <si>
+    <t>{"tag":{"id":408}}</t>
+  </si>
+  <si>
+    <t>{"errcode":1,"errmsg":"ok"}</t>
+  </si>
+  <si>
+    <t>{"grant_type":"client_credential","appid":"wx15938bc8b042cee0","secret":"f01c3e1836d6b40fb24db5dbc0142253"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求参数(get)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交数据(post)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{"tag" : {"name" : "衡东8888"}}</t>
-  </si>
-  <si>
-    <t>json键值对</t>
-  </si>
-  <si>
-    <t>{"errcode":45158}</t>
-  </si>
-  <si>
-    <t>case03</t>
-  </si>
-  <si>
-    <t>测试能否正确删除用户标签</t>
-  </si>
-  <si>
-    <t>删除标签接口</t>
-  </si>
-  <si>
-    <t>/cgi-bin/tags/delete</t>
-  </si>
-  <si>
-    <t>{"tag":{"id":408}}</t>
-  </si>
-  <si>
-    <t>{"errcode":1,"errmsg":"ok"}</t>
-  </si>
-  <si>
-    <t>{"grant_type":"client_credential","appid":"wx15938bc8b042cee0","secret":"f01c3e1836d6b40fb24db5dbc0142253"}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,7 +517,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -538,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -547,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -559,109 +562,109 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="O3" s="3"/>
     </row>
@@ -670,76 +673,76 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="O5" s="3"/>
     </row>
@@ -748,33 +751,33 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O6" s="3"/>
     </row>

</xml_diff>

<commit_message>
第十二次提交： samples/s1_demo.py importdata整合excel实战 common/requests_utils.py添加异常处理
</commit_message>
<xml_diff>
--- a/test_data/test_case.xlsx
+++ b/test_data/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharm\API_TEST_FRAME\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A62A10B-DF69-4DDA-AE4C-62FD13B87A55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88939B7-62A8-4848-BF42-B0D440B9E997}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>测试用例名称</t>
   </si>
@@ -168,6 +168,10 @@
   </si>
   <si>
     <t>{"tag" : {"name" : "衡东8888"}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.access_token</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -535,7 +539,7 @@
     <col min="11" max="11" width="16.796875" customWidth="1"/>
     <col min="12" max="12" width="22.8984375" customWidth="1"/>
     <col min="13" max="13" width="14.69921875" customWidth="1"/>
-    <col min="14" max="14" width="17.296875" customWidth="1"/>
+    <col min="14" max="14" width="27.796875" customWidth="1"/>
     <col min="15" max="15" width="23.09765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -658,7 +662,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>31</v>

</xml_diff>